<commit_message>
LV_TMTT0047023_VerifyFunctionalityOfRoundTripSectionOnCompanyInfoPage - Final - 30 Apr 2025
</commit_message>
<xml_diff>
--- a/TestData/LV_TMTT0047023_VerifyFunctionalityOfRoundTripSectionOnCompanyInfoPage.xlsx
+++ b/TestData/LV_TMTT0047023_VerifyFunctionalityOfRoundTripSectionOnCompanyInfoPage.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009BCEDF-ED14-478A-B9A0-718468E75E2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE1CE665-7170-4F09-9966-CB8378EC6CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3624" yWindow="1500" windowWidth="19416" windowHeight="10740" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
     <sheet name="ModuleName" sheetId="5" r:id="rId2"/>
     <sheet name="Company" sheetId="1" r:id="rId3"/>
-    <sheet name="CompanyRecordTypes" sheetId="3" r:id="rId4"/>
+    <sheet name="RoundTripFields" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>CompanyType</t>
   </si>
@@ -122,9 +122,6 @@
     <t>Postal Code</t>
   </si>
   <si>
-    <t>Company Record Types</t>
-  </si>
-  <si>
     <t>ModuleName</t>
   </si>
   <si>
@@ -156,6 +153,21 @@
   </si>
   <si>
     <t>TestCapitalProviderCompany</t>
+  </si>
+  <si>
+    <t>Round Trip Section Fields</t>
+  </si>
+  <si>
+    <t>Potential Round Trip</t>
+  </si>
+  <si>
+    <t>Round Trip Engagement</t>
+  </si>
+  <si>
+    <t>Round Trip Comment</t>
+  </si>
+  <si>
+    <t>Potential Round Trip Last Modified Date</t>
   </si>
 </sst>
 </file>
@@ -498,12 +510,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -527,12 +539,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -610,10 +622,10 @@
         <v>26</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
@@ -642,7 +654,7 @@
         <v>16</v>
       </c>
       <c r="I2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J2" t="s">
         <v>18</v>
@@ -657,13 +669,13 @@
         <v>24</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -671,7 +683,7 @@
         <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -693,30 +705,40 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="1" max="1" width="34.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LV_TMTT0047023_VerifyFunctionalityOfRoundTripSectionOnCompanyInfoPage - Initial - 1st May 2025
</commit_message>
<xml_diff>
--- a/TestData/LV_TMTT0047023_VerifyFunctionalityOfRoundTripSectionOnCompanyInfoPage.xlsx
+++ b/TestData/LV_TMTT0047023_VerifyFunctionalityOfRoundTripSectionOnCompanyInfoPage.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE1CE665-7170-4F09-9966-CB8378EC6CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A94DC1-8F55-43FE-A963-25C1032A8BBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3624" yWindow="1500" windowWidth="19416" windowHeight="10740" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3624" yWindow="1500" windowWidth="19416" windowHeight="10740" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
     <sheet name="ModuleName" sheetId="5" r:id="rId2"/>
     <sheet name="Company" sheetId="1" r:id="rId3"/>
     <sheet name="RoundTripFields" sheetId="3" r:id="rId4"/>
+    <sheet name="Tooltip" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>CompanyType</t>
   </si>
@@ -168,6 +169,12 @@
   </si>
   <si>
     <t>Potential Round Trip Last Modified Date</t>
+  </si>
+  <si>
+    <t>ToolTip Text</t>
+  </si>
+  <si>
+    <t>An engagement is typically considered a potential round trip if it is acquired by a sponsor (subject is a potential round trip) or by a sponsor-backed operating company (buyer is a potential round trip). Note "sponsor" includes firms tagged as Private Equity Group, Hedge Fund, or Family Office.</t>
   </si>
 </sst>
 </file>
@@ -211,11 +218,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -707,7 +717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -745,4 +755,32 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D595233-43AD-440D-9E59-397D7A136F04}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="57.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
1st May 2025 - Final Changes
</commit_message>
<xml_diff>
--- a/TestData/LV_TMTT0047023_VerifyFunctionalityOfRoundTripSectionOnCompanyInfoPage.xlsx
+++ b/TestData/LV_TMTT0047023_VerifyFunctionalityOfRoundTripSectionOnCompanyInfoPage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A94DC1-8F55-43FE-A963-25C1032A8BBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FDFE025-9B7A-450C-A063-F34F52D344E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3624" yWindow="1500" windowWidth="19416" windowHeight="10740" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3624" yWindow="1500" windowWidth="19416" windowHeight="10740" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Company" sheetId="1" r:id="rId3"/>
     <sheet name="RoundTripFields" sheetId="3" r:id="rId4"/>
     <sheet name="Tooltip" sheetId="6" r:id="rId5"/>
+    <sheet name="Warning" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>CompanyType</t>
   </si>
@@ -175,6 +176,12 @@
   </si>
   <si>
     <t>An engagement is typically considered a potential round trip if it is acquired by a sponsor (subject is a potential round trip) or by a sponsor-backed operating company (buyer is a potential round trip). Note "sponsor" includes firms tagged as Private Equity Group, Hedge Fund, or Family Office.</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>An asset is typically considered a potential round trip if it is an operating company acquired either by a private equity firm or by a PE-owned operating company. This company is not listed as an Operating Company that is PE-owned. If you still want to consider them a round trip candidate no change is needed; otherwise, please change the selection.</t>
   </si>
 </sst>
 </file>
@@ -761,7 +768,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D595233-43AD-440D-9E59-397D7A136F04}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -783,4 +790,32 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{763A622E-B657-4BEB-B238-35AFD2F494EC}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="97.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
LV_TMTT0047023_VerifyFunctionalityOfRoundTripSectionOnCompanyInfoPage - Initial - 2nd May 2025
</commit_message>
<xml_diff>
--- a/TestData/LV_TMTT0047023_VerifyFunctionalityOfRoundTripSectionOnCompanyInfoPage.xlsx
+++ b/TestData/LV_TMTT0047023_VerifyFunctionalityOfRoundTripSectionOnCompanyInfoPage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FDFE025-9B7A-450C-A063-F34F52D344E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D2CFD1C-4291-44A4-AD56-BAAE6CF62C0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3624" yWindow="1500" windowWidth="19416" windowHeight="10740" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="RoundTripFields" sheetId="3" r:id="rId4"/>
     <sheet name="Tooltip" sheetId="6" r:id="rId5"/>
     <sheet name="Warning" sheetId="7" r:id="rId6"/>
+    <sheet name="FlagReason" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t>CompanyType</t>
   </si>
@@ -182,6 +183,18 @@
   </si>
   <si>
     <t>An asset is typically considered a potential round trip if it is an operating company acquired either by a private equity firm or by a PE-owned operating company. This company is not listed as an Operating Company that is PE-owned. If you still want to consider them a round trip candidate no change is needed; otherwise, please change the selection.</t>
+  </si>
+  <si>
+    <t>Reason</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Request to Change Company Type</t>
+  </si>
+  <si>
+    <t>Requesting to either (i) change Company Type to Operating Company and Ownership to Private Equity Group or (ii) review the appropriateness of the round trip designation with CF operations</t>
   </si>
 </sst>
 </file>
@@ -225,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -233,6 +246,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -796,7 +818,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{763A622E-B657-4BEB-B238-35AFD2F494EC}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -818,4 +840,39 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A57591F-91BD-4ED7-BB91-C9F540592C06}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.44140625" customWidth="1"/>
+    <col min="2" max="2" width="56" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>